<commit_message>
prepost.dlcdefs: update test data, add rounding for robustness on tests
</commit_message>
<xml_diff>
--- a/wetb/prepost/tests/data/demo_dlc/source/htc/DLCs/dlc01_demos.xlsx
+++ b/wetb/prepost/tests/data/demo_dlc/source/htc/DLCs/dlc01_demos.xlsx
@@ -299,47 +299,49 @@
   </sheetPr>
   <dimension ref="A1:AM5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="18.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="38" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,21 +491,21 @@
         <v>0</v>
       </c>
       <c r="I2" s="7" t="n">
-        <f aca="false">(0.16*(0.75*E2+5.6))/E2</f>
+        <f aca="false">ROUND((0.16*(0.75*E2+5.6))/E2,4)</f>
         <v>0.232</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>40</v>
       </c>
       <c r="K2" s="8" t="n">
-        <f aca="false">E2*B2/8192</f>
-        <v>0.0390625</v>
+        <f aca="false">ROUND(E2*B2/8192, 5)</f>
+        <v>0.03906</v>
       </c>
       <c r="L2" s="5" t="n">
         <v>0</v>
       </c>
       <c r="M2" s="9" t="n">
-        <f aca="false">8/E2</f>
+        <f aca="false">ROUND(8/E2, 4)</f>
         <v>1</v>
       </c>
       <c r="N2" s="5" t="s">
@@ -601,22 +603,22 @@
         <v>0</v>
       </c>
       <c r="I3" s="7" t="n">
-        <f aca="false">(0.16*(0.75*E3+5.6))/E3</f>
-        <v>0.219555555555556</v>
+        <f aca="false">ROUND((0.16*(0.75*E3+5.6))/E3,4)</f>
+        <v>0.2196</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>40</v>
       </c>
       <c r="K3" s="8" t="n">
-        <f aca="false">E3*B3/8192</f>
-        <v>0.0439453125</v>
+        <f aca="false">ROUND(E3*B3/8192, 5)</f>
+        <v>0.04395</v>
       </c>
       <c r="L3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="M3" s="9" t="n">
-        <f aca="false">8/E3</f>
-        <v>0.888888888888889</v>
+        <f aca="false">ROUND(8/E3, 4)</f>
+        <v>0.8889</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>41</v>
@@ -713,21 +715,21 @@
         <v>1</v>
       </c>
       <c r="I4" s="7" t="n">
-        <f aca="false">(0.16*(0.75*E4+5.6))/E4</f>
+        <f aca="false">ROUND((0.16*(0.75*E4+5.6))/E4,4)</f>
         <v>0.2096</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>43</v>
       </c>
       <c r="K4" s="8" t="n">
-        <f aca="false">E4*B4/512</f>
+        <f aca="false">ROUND(E4*B4/512, 5)</f>
         <v>0.78125</v>
       </c>
       <c r="L4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="9" t="n">
-        <f aca="false">8/E4</f>
+        <f aca="false">ROUND(8/E4, 4)</f>
         <v>0.8</v>
       </c>
       <c r="N4" s="5" t="s">
@@ -825,22 +827,22 @@
         <v>1</v>
       </c>
       <c r="I5" s="7" t="n">
-        <f aca="false">(0.16*(0.75*E5+5.6))/E5</f>
-        <v>0.201454545454545</v>
+        <f aca="false">ROUND((0.16*(0.75*E5+5.6))/E5,4)</f>
+        <v>0.2015</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>44</v>
       </c>
       <c r="K5" s="8" t="n">
-        <f aca="false">E5*B5/512</f>
-        <v>0.859375</v>
+        <f aca="false">ROUND(E5*B5/512, 5)</f>
+        <v>0.85938</v>
       </c>
       <c r="L5" s="5" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="9" t="n">
-        <f aca="false">8/E5</f>
-        <v>0.727272727272727</v>
+        <f aca="false">ROUND(8/E5, 4)</f>
+        <v>0.7273</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
prepost: no more xls files, fix xlsx reference file
</commit_message>
<xml_diff>
--- a/wetb/prepost/tests/data/demo_dlc/source/htc/DLCs/dlc01_demos.xlsx
+++ b/wetb/prepost/tests/data/demo_dlc/source/htc/DLCs/dlc01_demos.xlsx
@@ -257,15 +257,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0000000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0"/>
-    <numFmt numFmtId="171" formatCode="0.00"/>
+    <numFmt numFmtId="168" formatCode="General"/>
+    <numFmt numFmtId="169" formatCode="0.0000000"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0"/>
+    <numFmt numFmtId="172" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -368,7 +369,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,7 +377,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,15 +385,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -409,17 +410,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ5"/>
+  <dimension ref="A1:BN5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.25"/>
@@ -445,7 +446,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="0" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="26.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="19.88"/>
@@ -458,7 +458,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="11.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="6.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="6.88"/>
@@ -482,10 +481,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="10.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="10.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="11.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="67" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,19 +682,6 @@
       <c r="BN1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="ALX1" s="0"/>
-      <c r="ALY1" s="0"/>
-      <c r="ALZ1" s="0"/>
-      <c r="AMA1" s="0"/>
-      <c r="AMB1" s="0"/>
-      <c r="AMC1" s="0"/>
-      <c r="AMD1" s="0"/>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="n">
@@ -1334,7 +1319,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>